<commit_message>
Changed circumference algorithm; Up dated data and images; Added cirfumference visualisation
</commit_message>
<xml_diff>
--- a/Data/data_IHPC_FFT.xlsx
+++ b/Data/data_IHPC_FFT.xlsx
@@ -53,6 +53,74 @@
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -413,7 +481,7 @@
         <v>23489</v>
       </c>
       <c r="C2" t="n">
-        <v>1669</v>
+        <v>1412.285482287407</v>
       </c>
       <c r="D2" t="n">
         <v>139.9390258789062</v>
@@ -445,7 +513,7 @@
         <v>126887</v>
       </c>
       <c r="C3" t="n">
-        <v>4473</v>
+        <v>3432.942671537399</v>
       </c>
       <c r="D3" t="n">
         <v>171.6033325195312</v>
@@ -465,7 +533,7 @@
         <v>14895</v>
       </c>
       <c r="C4" t="n">
-        <v>1166</v>
+        <v>872.6559777259827</v>
       </c>
       <c r="D4" t="n">
         <v>113.7035751342773</v>
@@ -485,7 +553,7 @@
         <v>56773</v>
       </c>
       <c r="C5" t="n">
-        <v>2790</v>
+        <v>1880.934319734573</v>
       </c>
       <c r="D5" t="n">
         <v>195.8195953369141</v>
@@ -505,7 +573,7 @@
         <v>7701</v>
       </c>
       <c r="C6" t="n">
-        <v>570</v>
+        <v>489.9726504087448</v>
       </c>
       <c r="D6" t="n">
         <v>85.38103485107422</v>
@@ -525,7 +593,7 @@
         <v>38520</v>
       </c>
       <c r="C7" t="n">
-        <v>2210</v>
+        <v>1847.478476047516</v>
       </c>
       <c r="D7" t="n">
         <v>97.80214691162109</v>
@@ -545,7 +613,7 @@
         <v>127734</v>
       </c>
       <c r="C8" t="n">
-        <v>3329</v>
+        <v>3115.232871055603</v>
       </c>
       <c r="D8" t="n">
         <v>158.8050079345703</v>
@@ -565,7 +633,7 @@
         <v>15948</v>
       </c>
       <c r="C9" t="n">
-        <v>1108</v>
+        <v>843.7859205007553</v>
       </c>
       <c r="D9" t="n">
         <v>77.46805572509766</v>
@@ -585,7 +653,7 @@
         <v>10121</v>
       </c>
       <c r="C10" t="n">
-        <v>682</v>
+        <v>578.9259679317474</v>
       </c>
       <c r="D10" t="n">
         <v>98.10954284667969</v>
@@ -605,7 +673,7 @@
         <v>27098</v>
       </c>
       <c r="C11" t="n">
-        <v>1885</v>
+        <v>1559.044929623604</v>
       </c>
       <c r="D11" t="n">
         <v>94.80092620849609</v>
@@ -625,7 +693,7 @@
         <v>12965</v>
       </c>
       <c r="C12" t="n">
-        <v>1043</v>
+        <v>856.4549672603607</v>
       </c>
       <c r="D12" t="n">
         <v>69.87619018554688</v>
@@ -645,7 +713,7 @@
         <v>31391</v>
       </c>
       <c r="C13" t="n">
-        <v>2280</v>
+        <v>1726.140382528305</v>
       </c>
       <c r="D13" t="n">
         <v>118.4514541625977</v>
@@ -665,7 +733,7 @@
         <v>88898</v>
       </c>
       <c r="C14" t="n">
-        <v>3981</v>
+        <v>2997.989354014397</v>
       </c>
       <c r="D14" t="n">
         <v>275.7662353515625</v>
@@ -685,7 +753,7 @@
         <v>9415</v>
       </c>
       <c r="C15" t="n">
-        <v>843</v>
+        <v>690.7320977449417</v>
       </c>
       <c r="D15" t="n">
         <v>87.38130187988281</v>
@@ -705,7 +773,7 @@
         <v>36582</v>
       </c>
       <c r="C16" t="n">
-        <v>2823</v>
+        <v>2322.757694482803</v>
       </c>
       <c r="D16" t="n">
         <v>186.0671997070312</v>
@@ -725,7 +793,7 @@
         <v>25451</v>
       </c>
       <c r="C17" t="n">
-        <v>1591</v>
+        <v>1313.966721653938</v>
       </c>
       <c r="D17" t="n">
         <v>116.950065612793</v>
@@ -745,7 +813,7 @@
         <v>30999</v>
       </c>
       <c r="C18" t="n">
-        <v>2083</v>
+        <v>1710.667293906212</v>
       </c>
       <c r="D18" t="n">
         <v>103.4430923461914</v>
@@ -765,7 +833,7 @@
         <v>7917</v>
       </c>
       <c r="C19" t="n">
-        <v>678</v>
+        <v>565.6366448402405</v>
       </c>
       <c r="D19" t="n">
         <v>64.07973480224609</v>
@@ -785,7 +853,7 @@
         <v>93394</v>
       </c>
       <c r="C20" t="n">
-        <v>5085</v>
+        <v>4006.544826507568</v>
       </c>
       <c r="D20" t="n">
         <v>281.6588745117188</v>
@@ -805,7 +873,7 @@
         <v>46514</v>
       </c>
       <c r="C21" t="n">
-        <v>2524</v>
+        <v>2114.723204612732</v>
       </c>
       <c r="D21" t="n">
         <v>86.75746154785156</v>
@@ -825,7 +893,7 @@
         <v>14721</v>
       </c>
       <c r="C22" t="n">
-        <v>1300</v>
+        <v>1070.989018917084</v>
       </c>
       <c r="D22" t="n">
         <v>114.6783676147461</v>
@@ -845,7 +913,7 @@
         <v>20253</v>
       </c>
       <c r="C23" t="n">
-        <v>1421</v>
+        <v>1182.385987520218</v>
       </c>
       <c r="D23" t="n">
         <v>68.26117706298828</v>
@@ -865,7 +933,7 @@
         <v>20163</v>
       </c>
       <c r="C24" t="n">
-        <v>1285</v>
+        <v>1089.366654634476</v>
       </c>
       <c r="D24" t="n">
         <v>72.34642791748047</v>
@@ -885,7 +953,7 @@
         <v>7811</v>
       </c>
       <c r="C25" t="n">
-        <v>728</v>
+        <v>597.5777697563171</v>
       </c>
       <c r="D25" t="n">
         <v>79.05519104003906</v>
@@ -905,7 +973,7 @@
         <v>27038</v>
       </c>
       <c r="C26" t="n">
-        <v>1295</v>
+        <v>1151.089524149895</v>
       </c>
       <c r="D26" t="n">
         <v>96.73746490478516</v>
@@ -925,7 +993,7 @@
         <v>26604</v>
       </c>
       <c r="C27" t="n">
-        <v>2174</v>
+        <v>1361.322060108185</v>
       </c>
       <c r="D27" t="n">
         <v>155.4207000732422</v>
@@ -945,7 +1013,7 @@
         <v>23789</v>
       </c>
       <c r="C28" t="n">
-        <v>1136</v>
+        <v>1044.923003554344</v>
       </c>
       <c r="D28" t="n">
         <v>107.7107086181641</v>
@@ -965,7 +1033,7 @@
         <v>15958</v>
       </c>
       <c r="C29" t="n">
-        <v>703</v>
+        <v>704.9503531455994</v>
       </c>
       <c r="D29" t="n">
         <v>111.2905654907227</v>
@@ -985,7 +1053,7 @@
         <v>8198</v>
       </c>
       <c r="C30" t="n">
-        <v>579</v>
+        <v>544.2396762371063</v>
       </c>
       <c r="D30" t="n">
         <v>58.04082107543945</v>

</xml_diff>